<commit_message>
Errores en la interfaz reparados
</commit_message>
<xml_diff>
--- a/bak_formato vacio.xlsx
+++ b/bak_formato vacio.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>carnet</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>scse.test1@gmail.com</t>
+  </si>
+  <si>
+    <t>Ingeniería civil</t>
+  </si>
+  <si>
+    <t>asdadsadsasd</t>
   </si>
 </sst>
 </file>
@@ -484,7 +490,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,8 +585,8 @@
       <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="7">
-        <v>33672</v>
+      <c r="F3" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>21</v>
@@ -614,7 +620,7 @@
         <v>26</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>